<commit_message>
Fix file test indicatori ISPRO SYT
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
@@ -380,13 +380,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,11 +748,11 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="P2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -865,7 +865,7 @@
         <v>68047648</v>
       </c>
       <c r="D5" s="10">
-        <v>551000000</v>
+        <v>551</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>1</v>
@@ -915,7 +915,7 @@
         <v>70206080</v>
       </c>
       <c r="D6" s="10">
-        <v>37000000</v>
+        <v>37</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>1</v>
@@ -967,7 +967,7 @@
         <v>81256270</v>
       </c>
       <c r="D7" s="10">
-        <v>234000000</v>
+        <v>234</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>1</v>
@@ -1067,11 +1067,11 @@
       </c>
       <c r="P11" s="15"/>
       <c r="Q11" s="16"/>
-      <c r="R11" s="19" t="s">
+      <c r="R11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
@@ -1138,7 +1138,7 @@
         <v>68047648</v>
       </c>
       <c r="D13" s="10">
-        <v>551000000</v>
+        <v>551</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>1</v>
@@ -1193,7 +1193,7 @@
         <v>70206080</v>
       </c>
       <c r="D14" s="10">
-        <v>37000000</v>
+        <v>37</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>1</v>
@@ -1250,7 +1250,7 @@
         <v>81256270</v>
       </c>
       <c r="D15" s="10">
-        <v>234000000</v>
+        <v>234</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>1</v>
@@ -1411,11 +1411,11 @@
       <c r="D20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="19" t="s">
+      <c r="N20" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
     </row>
@@ -1707,11 +1707,11 @@
       <c r="D29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U29" s="19" t="s">
+      <c r="U29" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="V29" s="19"/>
-      <c r="W29" s="19"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
@@ -2097,11 +2097,11 @@
       <c r="D38" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N38" s="19" t="s">
+      <c r="N38" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
@@ -2214,7 +2214,7 @@
       <c r="G41" s="10">
         <v>0.74209000000000003</v>
       </c>
-      <c r="H41" s="20">
+      <c r="H41" s="19">
         <v>1.7168680000000001</v>
       </c>
       <c r="I41" s="10">
@@ -2223,7 +2223,7 @@
       <c r="J41" s="17">
         <v>50</v>
       </c>
-      <c r="K41" s="20">
+      <c r="K41" s="19">
         <v>1.7168680000000001</v>
       </c>
       <c r="L41" s="10" t="s">
@@ -2304,7 +2304,7 @@
       <c r="G43" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="H43" s="21">
+      <c r="H43" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="I43" s="1">
@@ -2313,7 +2313,7 @@
       <c r="J43" s="18">
         <v>80</v>
       </c>
-      <c r="K43" s="21">
+      <c r="K43" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="L43" s="1" t="s">

</xml_diff>

<commit_message>
updatev retail e test ispr
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alberto.collu\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.monaco\Desktop\ISP\SorgentiGIT\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="CUSTOMER_TABLE_ESTERE SYT" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="84">
   <si>
     <t>SNDG</t>
   </si>
@@ -253,6 +253,30 @@
   </si>
   <si>
     <t>E0003E0002</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>E0002;E0003</t>
+  </si>
+  <si>
+    <t>ind_atteso</t>
+  </si>
+  <si>
+    <t>error_atteso</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>den errato</t>
+  </si>
+  <si>
+    <t>err_atteso</t>
   </si>
 </sst>
 </file>
@@ -262,8 +286,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -289,7 +313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +341,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,13 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -414,20 +444,26 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -754,47 +790,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="24.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="N2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O2" s="26"/>
+      <c r="T2"/>
+      <c r="U2"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
@@ -811,42 +838,38 @@
         <v>6</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="L3" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="M3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+    </row>
+    <row r="4" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="10">
@@ -862,43 +885,36 @@
         <v>6329</v>
       </c>
       <c r="G4" s="10">
-        <v>4644.2700000000004</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H4" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I4" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L4" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="10">
-        <v>68047613</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" s="4"/>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B5" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="10">
@@ -914,41 +930,37 @@
         <v>12742</v>
       </c>
       <c r="G5" s="10">
-        <v>13021</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H5" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I5" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J5" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L5" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M5" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="10">
-        <v>68047648</v>
-      </c>
-      <c r="Q5" s="10">
+      <c r="N5" s="10">
         <v>23.125226999999999</v>
       </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="6"/>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="O5" s="10"/>
+      <c r="P5" s="6"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B6" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="10">
@@ -964,43 +976,39 @@
         <v>10953</v>
       </c>
       <c r="G6" s="10">
-        <v>24307</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H6" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I6" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J6" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L6" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M6" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="10">
-        <v>70206080</v>
-      </c>
-      <c r="Q6" s="10">
+      <c r="N6" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="P6" s="6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B7" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="10">
@@ -1016,43 +1024,39 @@
         <v>95071</v>
       </c>
       <c r="G7" s="10">
-        <v>89548</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H7" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I7" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J7" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L7" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M7" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N7" s="10" t="s">
+      <c r="M7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="10">
-        <v>81256270</v>
-      </c>
-      <c r="Q7" s="10">
+      <c r="N7" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="O7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="S7" s="6"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="P7" s="6"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B8" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="10">
@@ -1068,41 +1072,37 @@
         <v>29839.56</v>
       </c>
       <c r="G8" s="10">
-        <v>4860.32</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H8" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I8" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J8" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L8" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M8" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N8" s="10" t="s">
+      <c r="M8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="10">
-        <v>81256680</v>
-      </c>
-      <c r="Q8" s="10">
+      <c r="N8" s="10">
         <v>2.7075819999999999</v>
       </c>
-      <c r="R8" s="10"/>
-      <c r="S8" s="6"/>
-    </row>
-    <row r="9" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="O8" s="10"/>
+      <c r="P8" s="6"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+    </row>
+    <row r="9" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="10">
@@ -1118,39 +1118,32 @@
         <v>15360776</v>
       </c>
       <c r="G9" s="10">
-        <v>13622001</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H9" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I9" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J9" s="10">
-        <v>0.27730519999999997</v>
+        <v>4949128</v>
       </c>
       <c r="K9" s="10">
-        <v>4949128</v>
+        <v>3.1037340000000002</v>
       </c>
       <c r="L9" s="10">
         <v>3.1037340000000002</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10">
         <v>3.1037340000000002</v>
       </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>3.1037340000000002</v>
-      </c>
-      <c r="R9" s="10"/>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="O9" s="10"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B10" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="10">
@@ -1166,39 +1159,35 @@
         <v>36277753.990000002</v>
       </c>
       <c r="G10" s="10">
-        <v>35186384</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H10" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I10" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J10" s="10">
-        <v>0.27730519999999997</v>
+        <v>22034940.920000002</v>
       </c>
       <c r="K10" s="10">
-        <v>22034940.920000002</v>
+        <v>1.646374</v>
       </c>
       <c r="L10" s="10">
         <v>1.646374</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="10"/>
+      <c r="N10" s="10">
         <v>1.646374</v>
       </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>1.646374</v>
-      </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="O10" s="10"/>
+      <c r="P10" s="6"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B11" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="10">
@@ -1214,39 +1203,35 @@
         <v>658673</v>
       </c>
       <c r="G11" s="10">
-        <v>1040863</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H11" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I11" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J11" s="10">
-        <v>0.27730519999999997</v>
+        <v>255297.5</v>
       </c>
       <c r="K11" s="10">
-        <v>255297.5</v>
+        <v>2.5800209999999999</v>
       </c>
       <c r="L11" s="10">
         <v>2.5800209999999999</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="10"/>
+      <c r="N11" s="10">
         <v>2.5800209999999999</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="Q11" s="10">
-        <v>2.5800209999999999</v>
-      </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="O11" s="10"/>
+      <c r="P11" s="6"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B12" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="10">
@@ -1262,39 +1247,35 @@
         <v>5140949</v>
       </c>
       <c r="G12" s="10">
-        <v>5214210</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H12" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I12" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J12" s="10">
-        <v>0.27730519999999997</v>
+        <v>2338974.5</v>
       </c>
       <c r="K12" s="10">
-        <v>2338974.5</v>
+        <v>2.1979500000000001</v>
       </c>
       <c r="L12" s="10">
         <v>2.1979500000000001</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="10"/>
+      <c r="N12" s="10">
         <v>2.1979500000000001</v>
       </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="Q12" s="10">
-        <v>2.1979500000000001</v>
-      </c>
-      <c r="R12" s="10"/>
-      <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="O12" s="10"/>
+      <c r="P12" s="6"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="10">
@@ -1310,39 +1291,35 @@
         <v>5030867</v>
       </c>
       <c r="G13" s="10">
-        <v>6492255</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H13" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I13" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J13" s="10">
-        <v>0.27730519999999997</v>
+        <v>669952</v>
       </c>
       <c r="K13" s="10">
-        <v>669952</v>
+        <v>7.5092949999999998</v>
       </c>
       <c r="L13" s="10">
         <v>7.5092949999999998</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="10"/>
+      <c r="N13" s="10">
         <v>7.5092949999999998</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>7.5092949999999998</v>
-      </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="O13" s="10"/>
+      <c r="P13" s="6"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+    </row>
+    <row r="14" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="10">
@@ -1357,44 +1334,37 @@
       <c r="F14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>1</v>
+      <c r="G14" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H14" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I14" s="10">
+      <c r="L14" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J14" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M14" s="10">
+      <c r="M14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="O14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="12"/>
-      <c r="P14" s="10">
-        <v>17962405</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B15" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="10">
@@ -1409,44 +1379,40 @@
       <c r="F15" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>1</v>
+      <c r="G15" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H15" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I15" s="10">
+      <c r="L15" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J15" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M15" s="10">
+      <c r="M15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N15" s="10" t="s">
+      <c r="O15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="12"/>
-      <c r="P15" s="10">
-        <v>48157476</v>
-      </c>
-      <c r="Q15" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S15" s="6"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="P15" s="6"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B16" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="10">
@@ -1461,44 +1427,40 @@
       <c r="F16" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>1</v>
+      <c r="G16" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H16" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I16" s="10">
+      <c r="L16" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J16" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M16" s="10">
+      <c r="M16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="O16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="12"/>
-      <c r="P16" s="10">
-        <v>59403681</v>
-      </c>
-      <c r="Q16" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+      <c r="P16" s="6"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B17" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="10">
@@ -1513,44 +1475,40 @@
       <c r="F17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>1</v>
+      <c r="G17" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H17" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I17" s="10">
+      <c r="L17" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J17" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M17" s="10">
+      <c r="M17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N17" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="O17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="12"/>
-      <c r="P17" s="10">
-        <v>70206081</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S17" s="6"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+      <c r="P17" s="6"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B18" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="10">
@@ -1565,55 +1523,51 @@
       <c r="F18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>1</v>
+      <c r="G18" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H18" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I18" s="10">
+      <c r="L18" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J18" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M18" s="10">
+      <c r="M18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="O18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O18" s="12"/>
-      <c r="P18" s="10">
-        <v>70206307</v>
-      </c>
-      <c r="Q18" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S18" s="6"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="P18" s="6"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="D21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="21" t="s">
+      <c r="P21" s="13"/>
+      <c r="Q21" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="R21" s="26"/>
+      <c r="T21"/>
+      <c r="U21"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1659,20 +1613,28 @@
       <c r="P22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" s="8" t="s">
+      <c r="Q22" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="T22" s="8" t="s">
+      <c r="R22" s="25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>53</v>
+      <c r="S22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T22" t="s">
+        <v>81</v>
+      </c>
+      <c r="U22" t="s">
+        <v>78</v>
+      </c>
+      <c r="V22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B23" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C23" s="10">
         <v>68047648</v>
@@ -1716,18 +1678,25 @@
       <c r="P23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="10">
-        <v>68047648</v>
-      </c>
-      <c r="S23" s="10">
+      <c r="Q23" s="10">
         <v>2.1466440000000002</v>
       </c>
-      <c r="T23" s="10"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
-        <v>53</v>
+      <c r="R23" s="10"/>
+      <c r="S23" s="2" t="e">
+        <f>G23/((D23+E23)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T23" s="2" t="e">
+        <f>H23/((E23+F23)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U23">
+        <v>0.96430340713054474</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C24" s="10">
         <v>70206080</v>
@@ -1771,20 +1740,30 @@
       <c r="P24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="10">
-        <v>70206080</v>
-      </c>
-      <c r="S24" s="10">
+      <c r="Q24" s="10">
         <v>11.508599999999999</v>
       </c>
-      <c r="T24" s="10" t="s">
+      <c r="R24" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
-        <v>53</v>
+      <c r="S24" s="2" t="e">
+        <f t="shared" ref="S24:S27" si="0">G24/((D24+E24)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T24" s="2" t="e">
+        <f t="shared" ref="T24:T27" si="1">H24/((E24+F24)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U24">
+        <v>11.508599999999999</v>
+      </c>
+      <c r="V24" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B25" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C25" s="10">
         <v>81256270</v>
@@ -1828,18 +1807,28 @@
       <c r="P25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="10">
-        <v>81256270</v>
-      </c>
-      <c r="S25" s="10">
+      <c r="Q25" s="10">
         <v>0.23152300000000001</v>
       </c>
-      <c r="T25" s="10"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>53</v>
+      <c r="R25" s="10"/>
+      <c r="S25" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T25" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U25">
+        <v>11.508599999999999</v>
+      </c>
+      <c r="V25" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B26" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C26" s="10">
         <v>81257338</v>
@@ -1883,18 +1872,25 @@
       <c r="P26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="10">
-        <v>81257338</v>
-      </c>
-      <c r="S26" s="10">
+      <c r="Q26" s="10">
         <v>2.8323559999999999</v>
       </c>
-      <c r="T26" s="10"/>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
-        <v>53</v>
+      <c r="R26" s="10"/>
+      <c r="S26" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T26" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U26">
+        <v>0.28449832433210331</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B27" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C27" s="10">
         <v>87962543</v>
@@ -1938,18 +1934,25 @@
       <c r="P27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="10">
-        <v>87962543</v>
-      </c>
-      <c r="S27" s="10">
+      <c r="Q27" s="10">
         <v>0.17911099999999999</v>
       </c>
-      <c r="T27" s="10"/>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
-        <v>53</v>
+      <c r="R27" s="10"/>
+      <c r="S27" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T27" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U27">
+        <v>-0.82824772620128728</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B28" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C28" s="10">
         <v>17959726</v>
@@ -1991,18 +1994,29 @@
         <v>1.811755</v>
       </c>
       <c r="P28" s="10"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="S28" s="10">
+      <c r="Q28" s="10">
         <v>1.811755</v>
       </c>
-      <c r="T28" s="10"/>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
-        <v>53</v>
+      <c r="R28" s="10"/>
+      <c r="S28" s="2">
+        <f t="shared" ref="S24:S37" si="2">G28/((D28+E28)/2)</f>
+        <v>3.1037338294746064</v>
+      </c>
+      <c r="T28" s="2">
+        <f>H28/((E28+F28)/2)</f>
+        <v>2.7131086947018033</v>
+      </c>
+      <c r="U28">
+        <f t="shared" ref="U24:U37" si="3">S28/T28-1</f>
+        <v>0.14397695733149996</v>
+      </c>
+      <c r="W28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B29" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C29" s="10">
         <v>17993020</v>
@@ -2044,18 +2058,29 @@
         <v>1.17293</v>
       </c>
       <c r="P29" s="10"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="S29" s="10">
+      <c r="Q29" s="10">
         <v>1.17293</v>
       </c>
-      <c r="T29" s="10"/>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
-        <v>53</v>
+      <c r="R29" s="10"/>
+      <c r="S29" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6463740076140854</v>
+      </c>
+      <c r="T29" s="2">
+        <f t="shared" ref="T24:T37" si="4">H29/((E29+F29)/2)</f>
+        <v>2.4036424369644163</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="3"/>
+        <v>-0.31505036593824354</v>
+      </c>
+      <c r="W29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B30" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C30" s="10">
         <v>26852786</v>
@@ -2097,18 +2122,29 @@
         <v>1.6497599999999999</v>
       </c>
       <c r="P30" s="10"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="S30" s="10">
+      <c r="Q30" s="10">
         <v>1.6497599999999999</v>
       </c>
-      <c r="T30" s="10"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
-        <v>53</v>
+      <c r="R30" s="10"/>
+      <c r="S30" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5800213476434357</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="4"/>
+        <v>2.5638771476652122</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="3"/>
+        <v>6.2967915576317424E-3</v>
+      </c>
+      <c r="W30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B31" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C31" s="10">
         <v>26852818</v>
@@ -2150,18 +2186,29 @@
         <v>1.7427950000000001</v>
       </c>
       <c r="P31" s="10"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="S31" s="10">
+      <c r="Q31" s="10">
         <v>1.7427950000000001</v>
       </c>
-      <c r="T31" s="10"/>
-    </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
-        <v>53</v>
+      <c r="R31" s="10"/>
+      <c r="S31" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1979499990273514</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2611642864447763</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="3"/>
+        <v>-2.7956521247209598E-2</v>
+      </c>
+      <c r="W31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B32" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C32" s="10">
         <v>26852821</v>
@@ -2203,17 +2250,28 @@
         <v>1.6762349999999999</v>
       </c>
       <c r="P32" s="10"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="S32" s="10">
+      <c r="Q32" s="10">
         <v>1.6762349999999999</v>
       </c>
-      <c r="T32" s="10"/>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+      <c r="R32" s="10"/>
+      <c r="S32" s="2">
+        <f t="shared" si="2"/>
+        <v>7.5092946957393965</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="4"/>
+        <v>5.4798569148401901</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="3"/>
+        <v>0.37034503134620467</v>
+      </c>
+      <c r="W32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B33" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="10">
@@ -2258,19 +2316,16 @@
       <c r="P33" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="10">
-        <v>17962405</v>
-      </c>
-      <c r="S33" s="10">
-        <v>0</v>
-      </c>
-      <c r="T33" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="14" t="s">
+      <c r="Q33" s="10">
+        <v>0</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U33"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B34" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="10">
@@ -2315,19 +2370,16 @@
       <c r="P34" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="10">
-        <v>48157476</v>
-      </c>
-      <c r="S34" s="10">
-        <v>0</v>
-      </c>
-      <c r="T34" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+      <c r="Q34" s="10">
+        <v>0</v>
+      </c>
+      <c r="R34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U34"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B35" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C35" s="10">
@@ -2372,19 +2424,16 @@
       <c r="P35" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="10">
-        <v>59403681</v>
-      </c>
-      <c r="S35" s="10">
-        <v>0</v>
-      </c>
-      <c r="T35" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="Q35" s="10">
+        <v>0</v>
+      </c>
+      <c r="R35" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U35"/>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B36" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C36" s="10">
@@ -2429,19 +2478,16 @@
       <c r="P36" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="10">
-        <v>70206081</v>
-      </c>
-      <c r="S36" s="10">
-        <v>0</v>
-      </c>
-      <c r="T36" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+      <c r="Q36" s="10">
+        <v>0</v>
+      </c>
+      <c r="R36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U36"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B37" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C37" s="10">
@@ -2486,30 +2532,28 @@
       <c r="P37" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="10">
-        <v>70206307</v>
-      </c>
-      <c r="S37" s="10">
-        <v>0</v>
-      </c>
-      <c r="T37" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="Q37" s="10">
+        <v>0</v>
+      </c>
+      <c r="R37" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U37"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D40" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N40" s="21" t="s">
+      <c r="M40" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="16"/>
-      <c r="R40" s="16"/>
-    </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N40" s="26"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="T40"/>
+      <c r="U40"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
         <v>16</v>
       </c>
@@ -2543,21 +2587,19 @@
       <c r="L41" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M41" s="11"/>
-      <c r="N41" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O41" s="8" t="s">
+      <c r="M41" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="P41" s="8" t="s">
+      <c r="N41" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="T41"/>
+      <c r="U41"/>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B42" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C42" s="10">
@@ -2590,19 +2632,17 @@
       <c r="L42" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M42" s="11"/>
-      <c r="N42" s="10">
-        <v>27541053</v>
-      </c>
-      <c r="O42" s="10">
+      <c r="M42" s="10">
         <v>2.693085</v>
       </c>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="14" t="s">
+      <c r="N42" s="10"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="T42"/>
+      <c r="U42"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B43" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C43" s="10">
@@ -2635,19 +2675,17 @@
       <c r="L43" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="10">
-        <v>34457908</v>
-      </c>
-      <c r="O43" s="10">
+      <c r="M43" s="10">
         <v>105.300326</v>
       </c>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+      <c r="N43" s="10"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="T43"/>
+      <c r="U43"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B44" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="10">
@@ -2680,19 +2718,17 @@
       <c r="L44" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M44" s="11"/>
-      <c r="N44" s="10">
-        <v>52866669</v>
-      </c>
-      <c r="O44" s="10">
+      <c r="M44" s="10">
         <v>32.541947999999998</v>
       </c>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
+      <c r="N44" s="10"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="T44"/>
+      <c r="U44"/>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B45" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C45" s="10">
@@ -2725,19 +2761,17 @@
       <c r="L45" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M45" s="11"/>
-      <c r="N45" s="10">
-        <v>68047255</v>
-      </c>
-      <c r="O45" s="10">
+      <c r="M45" s="10">
         <v>3.2832210000000002</v>
       </c>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B46" s="14" t="s">
+      <c r="N45" s="10"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="T45"/>
+      <c r="U45"/>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B46" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="10">
@@ -2770,21 +2804,19 @@
       <c r="L46" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M46" s="11"/>
-      <c r="N46" s="10">
-        <v>68047613</v>
-      </c>
-      <c r="O46" s="10">
+      <c r="M46" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P46" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-    </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
+      <c r="N46" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="T46"/>
+      <c r="U46"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B47" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C47" s="10">
@@ -2815,19 +2847,17 @@
         <v>3.3743629999999998</v>
       </c>
       <c r="L47" s="10"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="O47" s="10">
+      <c r="M47" s="10">
         <v>3.3743629999999998</v>
       </c>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-    </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+      <c r="N47" s="10"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="T47"/>
+      <c r="U47"/>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B48" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C48" s="10">
@@ -2858,19 +2888,17 @@
         <v>6.3879580000000002</v>
       </c>
       <c r="L48" s="10"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="O48" s="10">
+      <c r="M48" s="10">
         <v>6.3879580000000002</v>
       </c>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
+      <c r="N48" s="10"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="T48"/>
+      <c r="U48"/>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B49" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C49" s="10">
@@ -2901,19 +2929,17 @@
         <v>2.5449679999999999</v>
       </c>
       <c r="L49" s="10"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="O49" s="10">
+      <c r="M49" s="10">
         <v>2.5449679999999999</v>
       </c>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-    </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
+      <c r="N49" s="10"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="T49"/>
+      <c r="U49"/>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B50" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="10">
@@ -2944,19 +2970,17 @@
         <v>14.894848</v>
       </c>
       <c r="L50" s="10"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="O50" s="10">
+      <c r="M50" s="10">
         <v>14.894848</v>
       </c>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-    </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
+      <c r="N50" s="10"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="T50"/>
+      <c r="U50"/>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B51" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C51" s="10">
@@ -2987,19 +3011,19 @@
         <v>3.6481370000000002</v>
       </c>
       <c r="L51" s="10"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="O51" s="10">
+      <c r="M51" s="10">
         <v>3.6481370000000002</v>
       </c>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-    </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="14"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="T51"/>
+      <c r="U51"/>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B52" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C52" s="10">
         <v>17962405</v>
       </c>
@@ -3030,21 +3054,21 @@
       <c r="L52" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M52" s="11"/>
-      <c r="N52" s="10">
-        <v>17962405</v>
-      </c>
-      <c r="O52" s="10">
+      <c r="M52" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P52" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-    </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B53" s="14"/>
+      <c r="N52" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="T52"/>
+      <c r="U52"/>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B53" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C53" s="10">
         <v>48157476</v>
       </c>
@@ -3075,21 +3099,21 @@
       <c r="L53" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M53" s="11"/>
-      <c r="N53" s="10">
-        <v>48157476</v>
-      </c>
-      <c r="O53" s="10">
+      <c r="M53" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P53" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-    </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="14"/>
+      <c r="N53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="T53"/>
+      <c r="U53"/>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B54" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C54" s="10">
         <v>59403681</v>
       </c>
@@ -3120,21 +3144,21 @@
       <c r="L54" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M54" s="11"/>
-      <c r="N54" s="10">
-        <v>59403681</v>
-      </c>
-      <c r="O54" s="10">
+      <c r="M54" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P54" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="11"/>
-    </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B55" s="14"/>
+      <c r="N54" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="T54"/>
+      <c r="U54"/>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B55" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C55" s="10">
         <v>68047257</v>
       </c>
@@ -3165,21 +3189,21 @@
       <c r="L55" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M55" s="11"/>
-      <c r="N55" s="10">
-        <v>68047257</v>
-      </c>
-      <c r="O55" s="10">
+      <c r="M55" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P55" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-    </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="14"/>
+      <c r="N55" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="T55"/>
+      <c r="U55"/>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B56" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C56" s="10">
         <v>70206081</v>
       </c>
@@ -3210,40 +3234,37 @@
       <c r="L56" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M56" s="11"/>
-      <c r="N56" s="10">
-        <v>70206081</v>
-      </c>
-      <c r="O56" s="10">
+      <c r="M56" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P56" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-    </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="T56"/>
+      <c r="U56"/>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.3">
       <c r="P57" s="5"/>
       <c r="Q57" s="5"/>
       <c r="R57" s="5"/>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.3">
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
       <c r="R58" s="5"/>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D59" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U59" s="21" t="s">
+      <c r="T59" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="V59" s="21"/>
-      <c r="W59" s="21"/>
-    </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U59" s="26"/>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B60" s="9" t="s">
         <v>16</v>
       </c>
@@ -3298,18 +3319,15 @@
       <c r="S60" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="U60" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V60" s="8" t="s">
+      <c r="T60" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="W60" s="8" t="s">
+      <c r="U60" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B61" s="14" t="s">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B61" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C61" s="10">
@@ -3363,16 +3381,13 @@
       <c r="S61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U61" s="10">
-        <v>27541053</v>
-      </c>
-      <c r="V61" s="10">
+      <c r="T61" s="10">
         <v>-0.86645000000000005</v>
       </c>
-      <c r="W61" s="10"/>
-    </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B62" s="14" t="s">
+      <c r="U61" s="10"/>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B62" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C62" s="10">
@@ -3426,16 +3441,13 @@
       <c r="S62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U62" s="10">
-        <v>70206124</v>
-      </c>
-      <c r="V62" s="10">
+      <c r="T62" s="10">
         <v>-0.88441499999999995</v>
       </c>
-      <c r="W62" s="10"/>
-    </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B63" s="14" t="s">
+      <c r="U62" s="10"/>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B63" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C63" s="10">
@@ -3489,16 +3501,13 @@
       <c r="S63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U63" s="10">
-        <v>81256268</v>
-      </c>
-      <c r="V63" s="10">
+      <c r="T63" s="10">
         <v>1.743474</v>
       </c>
-      <c r="W63" s="10"/>
-    </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B64" s="14" t="s">
+      <c r="U63" s="10"/>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B64" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C64" s="10">
@@ -3552,16 +3561,13 @@
       <c r="S64" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U64" s="10">
-        <v>81256616</v>
-      </c>
-      <c r="V64" s="10">
+      <c r="T64" s="10">
         <v>12.61281</v>
       </c>
-      <c r="W64" s="10"/>
-    </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B65" s="14" t="s">
+      <c r="U64" s="10"/>
+    </row>
+    <row r="65" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B65" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C65" s="10">
@@ -3615,16 +3621,13 @@
       <c r="S65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U65" s="10">
-        <v>81256724</v>
-      </c>
-      <c r="V65" s="10">
+      <c r="T65" s="10">
         <v>1.225859</v>
       </c>
-      <c r="W65" s="10"/>
-    </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B66" s="14" t="s">
+      <c r="U65" s="10"/>
+    </row>
+    <row r="66" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B66" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C66" s="10">
@@ -3676,16 +3679,13 @@
         <v>0.81800799999999996</v>
       </c>
       <c r="S66" s="1"/>
-      <c r="U66" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="V66" s="1">
+      <c r="T66" s="1">
         <v>0.81800799999999996</v>
       </c>
-      <c r="W66" s="1"/>
-    </row>
-    <row r="67" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B67" s="14" t="s">
+      <c r="U66" s="1"/>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B67" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C67" s="10">
@@ -3737,16 +3737,13 @@
         <v>0.12714</v>
       </c>
       <c r="S67" s="1"/>
-      <c r="U67" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="V67" s="1">
+      <c r="T67" s="1">
         <v>0.12714</v>
       </c>
-      <c r="W67" s="1"/>
-    </row>
-    <row r="68" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B68" s="14" t="s">
+      <c r="U67" s="1"/>
+    </row>
+    <row r="68" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B68" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C68" s="10">
@@ -3798,16 +3795,13 @@
         <v>-0.396013</v>
       </c>
       <c r="S68" s="1"/>
-      <c r="U68" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="V68" s="1">
+      <c r="T68" s="1">
         <v>-0.396013</v>
       </c>
-      <c r="W68" s="1"/>
-    </row>
-    <row r="69" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B69" s="14" t="s">
+      <c r="U68" s="1"/>
+    </row>
+    <row r="69" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B69" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C69" s="10">
@@ -3859,16 +3853,13 @@
         <v>0.27766600000000002</v>
       </c>
       <c r="S69" s="1"/>
-      <c r="U69" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="V69" s="1">
+      <c r="T69" s="1">
         <v>0.27766600000000002</v>
       </c>
-      <c r="W69" s="1"/>
-    </row>
-    <row r="70" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B70" s="14" t="s">
+      <c r="U69" s="1"/>
+    </row>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B70" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C70" s="10">
@@ -3920,25 +3911,22 @@
         <v>0.262847</v>
       </c>
       <c r="S70" s="1"/>
-      <c r="U70" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="V70" s="1">
+      <c r="T70" s="1">
         <v>0.262847</v>
       </c>
-      <c r="W70" s="1"/>
-    </row>
-    <row r="71" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B71" s="14" t="s">
+      <c r="U70" s="1"/>
+    </row>
+    <row r="71" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B71" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C71" s="10">
         <v>27853141</v>
       </c>
-      <c r="D71" s="25">
+      <c r="D71" s="22">
         <v>92858</v>
       </c>
-      <c r="E71" s="25">
+      <c r="E71" s="22">
         <v>96325</v>
       </c>
       <c r="F71" s="10" t="s">
@@ -3956,22 +3944,22 @@
       <c r="J71" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K71" s="26">
+      <c r="K71" s="23">
         <v>92858</v>
       </c>
-      <c r="L71" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M71" s="26">
+      <c r="L71" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M71" s="23">
         <v>96325</v>
       </c>
-      <c r="N71" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O71" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P71" s="27" t="s">
+      <c r="N71" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O71" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P71" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q71" s="1">
@@ -3980,30 +3968,27 @@
       <c r="R71" s="1">
         <v>0</v>
       </c>
-      <c r="S71" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U71" s="10">
-        <v>27853141</v>
-      </c>
-      <c r="V71" s="1">
-        <v>0</v>
-      </c>
-      <c r="W71" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B72" s="14" t="s">
+      <c r="S71" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T71" s="1">
+        <v>0</v>
+      </c>
+      <c r="U71" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B72" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C72" s="10">
         <v>27853308</v>
       </c>
-      <c r="D72" s="25">
+      <c r="D72" s="22">
         <v>224506</v>
       </c>
-      <c r="E72" s="25">
+      <c r="E72" s="22">
         <v>146182</v>
       </c>
       <c r="F72" s="10" t="s">
@@ -4021,22 +4006,22 @@
       <c r="J72" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K72" s="26">
+      <c r="K72" s="23">
         <v>224506</v>
       </c>
-      <c r="L72" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M72" s="26">
+      <c r="L72" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M72" s="23">
         <v>146182</v>
       </c>
-      <c r="N72" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O72" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P72" s="27" t="s">
+      <c r="N72" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O72" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P72" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q72" s="1">
@@ -4045,30 +4030,27 @@
       <c r="R72" s="1">
         <v>0</v>
       </c>
-      <c r="S72" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U72" s="10">
-        <v>27853308</v>
-      </c>
-      <c r="V72" s="1">
-        <v>0</v>
-      </c>
-      <c r="W72" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B73" s="14" t="s">
+      <c r="S72" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T72" s="1">
+        <v>0</v>
+      </c>
+      <c r="U72" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B73" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C73" s="10">
         <v>68047770</v>
       </c>
-      <c r="D73" s="25">
+      <c r="D73" s="22">
         <v>1678951</v>
       </c>
-      <c r="E73" s="25">
+      <c r="E73" s="22">
         <v>1408373</v>
       </c>
       <c r="F73" s="10" t="s">
@@ -4086,22 +4068,22 @@
       <c r="J73" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K73" s="26">
+      <c r="K73" s="23">
         <v>1678951</v>
       </c>
-      <c r="L73" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M73" s="26">
+      <c r="L73" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M73" s="23">
         <v>1408373</v>
       </c>
-      <c r="N73" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O73" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P73" s="27" t="s">
+      <c r="N73" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O73" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P73" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q73" s="1">
@@ -4110,30 +4092,27 @@
       <c r="R73" s="1">
         <v>0</v>
       </c>
-      <c r="S73" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U73" s="10">
-        <v>68047770</v>
-      </c>
-      <c r="V73" s="1">
-        <v>0</v>
-      </c>
-      <c r="W73" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B74" s="14" t="s">
+      <c r="S73" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T73" s="1">
+        <v>0</v>
+      </c>
+      <c r="U73" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B74" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C74" s="10">
         <v>68048348</v>
       </c>
-      <c r="D74" s="25">
+      <c r="D74" s="22">
         <v>32873</v>
       </c>
-      <c r="E74" s="25">
+      <c r="E74" s="22">
         <v>45195.5</v>
       </c>
       <c r="F74" s="10" t="s">
@@ -4151,22 +4130,22 @@
       <c r="J74" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K74" s="26">
+      <c r="K74" s="23">
         <v>32873</v>
       </c>
-      <c r="L74" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M74" s="26">
+      <c r="L74" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M74" s="23">
         <v>45195.5</v>
       </c>
-      <c r="N74" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O74" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P74" s="27" t="s">
+      <c r="N74" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O74" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P74" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q74" s="1">
@@ -4175,30 +4154,27 @@
       <c r="R74" s="1">
         <v>0</v>
       </c>
-      <c r="S74" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U74" s="10">
-        <v>68048348</v>
-      </c>
-      <c r="V74" s="1">
-        <v>0</v>
-      </c>
-      <c r="W74" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B75" s="14" t="s">
+      <c r="S74" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T74" s="1">
+        <v>0</v>
+      </c>
+      <c r="U74" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B75" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C75" s="10">
         <v>81256246</v>
       </c>
-      <c r="D75" s="25">
+      <c r="D75" s="22">
         <v>364466</v>
       </c>
-      <c r="E75" s="25">
+      <c r="E75" s="22">
         <v>269600</v>
       </c>
       <c r="F75" s="10" t="s">
@@ -4216,22 +4192,22 @@
       <c r="J75" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K75" s="26">
+      <c r="K75" s="23">
         <v>364466</v>
       </c>
-      <c r="L75" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M75" s="26">
+      <c r="L75" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M75" s="23">
         <v>269600</v>
       </c>
-      <c r="N75" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O75" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P75" s="27" t="s">
+      <c r="N75" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O75" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P75" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q75" s="1">
@@ -4240,30 +4216,28 @@
       <c r="R75" s="1">
         <v>0</v>
       </c>
-      <c r="S75" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U75" s="10">
-        <v>81256246</v>
-      </c>
-      <c r="V75" s="1">
-        <v>0</v>
-      </c>
-      <c r="W75" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="S75" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T75" s="1">
+        <v>0</v>
+      </c>
+      <c r="U75" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N78" s="21" t="s">
+      <c r="M78" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="O78" s="21"/>
-      <c r="P78" s="21"/>
-    </row>
-    <row r="79" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N78" s="26"/>
+      <c r="T78"/>
+      <c r="U78"/>
+    </row>
+    <row r="79" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B79" s="9" t="s">
         <v>16</v>
       </c>
@@ -4297,36 +4271,36 @@
       <c r="L79" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="M79" s="11"/>
-      <c r="N79" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O79" s="8" t="s">
+      <c r="M79" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="P79" s="8" t="s">
+      <c r="N79" s="25" t="s">
         <v>62</v>
       </c>
+      <c r="O79" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="P79" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="Q79" s="11"/>
-      <c r="R79" s="11"/>
-      <c r="S79" s="11"/>
-    </row>
-    <row r="80" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B80" s="14" t="s">
-        <v>53</v>
+      <c r="T79"/>
+      <c r="U79"/>
+    </row>
+    <row r="80" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B80" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D80" s="17">
+      <c r="D80" s="15">
         <v>10</v>
       </c>
-      <c r="E80" s="17">
+      <c r="E80" s="15">
         <v>500</v>
       </c>
-      <c r="F80" s="10" t="s">
-        <v>1</v>
-      </c>
+      <c r="F80" s="10"/>
       <c r="G80" s="10">
         <v>0.74209000000000003</v>
       </c>
@@ -4336,87 +4310,90 @@
       <c r="I80" s="10">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J80" s="17">
+      <c r="J80" s="15">
         <v>50</v>
       </c>
-      <c r="K80" s="17">
+      <c r="K80" s="15">
         <v>50</v>
       </c>
       <c r="L80" s="10"/>
-      <c r="M80" s="11"/>
-      <c r="N80" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="O80" s="10">
+      <c r="M80" s="10">
         <v>50</v>
       </c>
-      <c r="P80" s="10"/>
+      <c r="N80" s="10"/>
+      <c r="O80" s="5">
+        <f>(E80+F80)/D80</f>
+        <v>50</v>
+      </c>
+      <c r="P80" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-      <c r="S80" s="5"/>
-    </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B81" s="14" t="s">
-        <v>53</v>
+      <c r="T80"/>
+      <c r="U80"/>
+    </row>
+    <row r="81" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B81" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D81" s="17">
+      <c r="D81" s="15">
         <v>10</v>
       </c>
-      <c r="E81" s="17">
+      <c r="E81" s="15">
         <v>500</v>
       </c>
-      <c r="F81" s="10" t="s">
-        <v>1</v>
-      </c>
+      <c r="F81" s="10"/>
       <c r="G81" s="10">
         <v>0.74209000000000003</v>
       </c>
-      <c r="H81" s="19">
+      <c r="H81" s="17">
         <v>1.7168680000000001</v>
       </c>
       <c r="I81" s="10">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J81" s="17">
+      <c r="J81" s="15">
         <v>50</v>
       </c>
-      <c r="K81" s="19">
+      <c r="K81" s="17">
         <v>1.7168680000000001</v>
       </c>
       <c r="L81" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="M81" s="11"/>
+      <c r="M81" s="10">
+        <v>1.7168680000000001</v>
+      </c>
       <c r="N81" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="O81" s="10">
+        <v>68</v>
+      </c>
+      <c r="O81" s="5">
         <v>1.7168680000000001</v>
       </c>
       <c r="P81" s="10" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
-      <c r="S81" s="5"/>
-    </row>
-    <row r="82" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B82" s="10" t="s">
+      <c r="T81"/>
+      <c r="U81"/>
+    </row>
+    <row r="82" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B82" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D82" s="17">
+      <c r="D82" s="15">
         <v>10</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F82" s="18">
+      <c r="F82" s="16">
         <v>800</v>
       </c>
       <c r="G82" s="1">
@@ -4428,70 +4405,75 @@
       <c r="I82" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J82" s="18">
+      <c r="J82" s="16">
         <v>80</v>
       </c>
-      <c r="K82" s="18">
+      <c r="K82" s="16">
         <v>80</v>
       </c>
       <c r="L82" s="1"/>
-      <c r="N82" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="O82" s="1">
+      <c r="M82" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="P82" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B83" s="10" t="s">
-        <v>53</v>
+      <c r="N82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O82" s="5"/>
+      <c r="T82"/>
+      <c r="U82"/>
+    </row>
+    <row r="83" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B83" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D83" s="17">
+      <c r="D83" s="15">
         <v>10</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F83" s="18">
+      <c r="F83" s="16">
         <v>800</v>
       </c>
       <c r="G83" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="H83" s="20">
+      <c r="H83" s="18">
         <v>1.7168680000000001</v>
       </c>
       <c r="I83" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J83" s="18">
+      <c r="J83" s="16">
         <v>80</v>
       </c>
-      <c r="K83" s="20">
+      <c r="K83" s="18">
         <v>1.7168680000000001</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N83" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="O83" s="1">
+      <c r="M83" s="1">
         <v>0.74209000000000003</v>
       </c>
+      <c r="N83" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O83" s="5">
+        <v>0.74209000000000003</v>
+      </c>
       <c r="P83" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B84" s="10" t="s">
-        <v>53</v>
+        <v>2</v>
+      </c>
+      <c r="T83"/>
+      <c r="U83"/>
+    </row>
+    <row r="84" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B84" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>69</v>
@@ -4523,19 +4505,19 @@
       <c r="L84" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N84" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="O84" s="1">
+      <c r="M84" s="1">
         <v>1.7168680000000001</v>
       </c>
-      <c r="P84" s="1" t="s">
+      <c r="N84" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B85" s="10" t="s">
-        <v>53</v>
+      <c r="O84" s="5"/>
+      <c r="T84"/>
+      <c r="U84"/>
+    </row>
+    <row r="85" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B85" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>70</v>
@@ -4567,18 +4549,18 @@
       <c r="L85" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N85" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="O85" s="1">
+      <c r="M85" s="1">
         <v>1.7168680000000001</v>
       </c>
-      <c r="P85" s="1" t="s">
+      <c r="N85" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B86" s="10" t="s">
+      <c r="O85" s="5"/>
+      <c r="T85"/>
+      <c r="U85"/>
+    </row>
+    <row r="86" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B86" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -4611,18 +4593,18 @@
       <c r="L86" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N86" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O86" s="1">
+      <c r="M86" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="P86" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B87" s="10" t="s">
+      <c r="N86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O86" s="5"/>
+      <c r="T86"/>
+      <c r="U86"/>
+    </row>
+    <row r="87" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B87" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -4655,32 +4637,30 @@
       <c r="L87" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N87" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O87" s="1">
+      <c r="M87" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="P87" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B88" s="10" t="s">
-        <v>53</v>
+      <c r="N87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O87" s="5"/>
+      <c r="T87"/>
+      <c r="U87"/>
+    </row>
+    <row r="88" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B88" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D88" s="18">
+      <c r="D88" s="16">
         <v>500</v>
       </c>
-      <c r="E88" s="18">
+      <c r="E88" s="16">
         <v>10</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="F88" s="1"/>
       <c r="G88" s="1">
         <v>0.74209000000000003</v>
       </c>
@@ -4690,7 +4670,7 @@
       <c r="I88" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J88" s="18">
+      <c r="J88" s="16">
         <v>50</v>
       </c>
       <c r="K88" s="1">
@@ -4699,32 +4679,35 @@
       <c r="L88" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N88" s="10" t="s">
-        <v>73</v>
+      <c r="M88" s="1">
+        <v>1.7168680000000001</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="O88" s="1">
-        <v>1.7168680000000001</v>
-      </c>
-      <c r="P88" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B89" s="10" t="s">
-        <v>53</v>
+        <v>6.9793999999999995E-2</v>
+      </c>
+      <c r="P88" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="T88"/>
+      <c r="U88"/>
+    </row>
+    <row r="89" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B89" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D89" s="18">
+      <c r="D89" s="16">
         <v>500</v>
       </c>
-      <c r="E89" s="18">
+      <c r="E89" s="16">
         <v>10</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="F89" s="1"/>
       <c r="G89" s="1">
         <v>0.74209000000000003</v>
       </c>
@@ -4734,7 +4717,7 @@
       <c r="I89" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J89" s="18">
+      <c r="J89" s="16">
         <v>50</v>
       </c>
       <c r="K89" s="1">
@@ -4743,23 +4726,28 @@
       <c r="L89" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N89" s="10" t="s">
-        <v>74</v>
+      <c r="M89" s="1">
+        <v>1.7168680000000001</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="O89" s="1">
-        <v>1.7168680000000001</v>
-      </c>
-      <c r="P89" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>6.9793999999999995E-2</v>
+      </c>
+      <c r="P89" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="T89"/>
+      <c r="U89"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="U59:W59"/>
-    <mergeCell ref="N78:P78"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="T59:U59"/>
+    <mergeCell ref="M78:N78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4774,226 +4762,226 @@
       <selection activeCell="B3" sqref="B3:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="19">
         <v>500</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="19">
         <v>10</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="19">
         <v>800</v>
       </c>
       <c r="F3">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H3">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="19">
         <v>130</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="K3" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="19">
         <v>500</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="19">
         <v>10</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="19">
         <v>800</v>
       </c>
       <c r="F4">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H4">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="19">
         <v>130</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="19">
         <v>500</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="19">
         <v>10</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="19">
         <v>800</v>
       </c>
       <c r="F5">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H5">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="19">
         <v>130</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="19">
         <v>500</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="19">
         <v>10</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="19">
         <v>800</v>
       </c>
       <c r="F6">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H6">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="19">
         <v>130</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="K6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="19">
         <v>500</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="19">
         <v>10</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="19">
         <v>800</v>
       </c>
       <c r="F7">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H7">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="19">
         <v>130</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed ind 73  aggiornato file test_ind_ISPRO_syt
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="83">
   <si>
     <t>SNDG</t>
   </si>
@@ -253,6 +253,27 @@
   </si>
   <si>
     <t>E0003E0002</t>
+  </si>
+  <si>
+    <t>E0002;E0003</t>
+  </si>
+  <si>
+    <t>ind_atteso</t>
+  </si>
+  <si>
+    <t>error_atteso</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>den errato</t>
+  </si>
+  <si>
+    <t>err_atteso</t>
   </si>
 </sst>
 </file>
@@ -262,8 +283,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -289,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,13 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -414,19 +435,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -754,45 +778,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="N2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
+      <c r="O2" s="26"/>
+      <c r="T2"/>
+      <c r="U2"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -811,42 +836,38 @@
         <v>6</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="L3" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="M3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
     </row>
     <row r="4" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="10">
@@ -862,43 +883,36 @@
         <v>6329</v>
       </c>
       <c r="G4" s="10">
-        <v>4644.2700000000004</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H4" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I4" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L4" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="10">
-        <v>68047613</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" s="4"/>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="10">
@@ -914,41 +928,37 @@
         <v>12742</v>
       </c>
       <c r="G5" s="10">
-        <v>13021</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H5" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I5" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J5" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L5" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M5" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="10">
-        <v>68047648</v>
-      </c>
-      <c r="Q5" s="10">
+      <c r="N5" s="10">
         <v>23.125226999999999</v>
       </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="6"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="6"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="10">
@@ -964,43 +974,39 @@
         <v>10953</v>
       </c>
       <c r="G6" s="10">
-        <v>24307</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H6" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I6" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J6" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L6" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M6" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="10">
-        <v>70206080</v>
-      </c>
-      <c r="Q6" s="10">
+      <c r="N6" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="S6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="10">
@@ -1016,43 +1022,39 @@
         <v>95071</v>
       </c>
       <c r="G7" s="10">
-        <v>89548</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H7" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I7" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J7" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L7" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M7" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N7" s="10" t="s">
+      <c r="M7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="10">
-        <v>81256270</v>
-      </c>
-      <c r="Q7" s="10">
+      <c r="N7" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="O7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="S7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="10">
@@ -1068,41 +1070,37 @@
         <v>29839.56</v>
       </c>
       <c r="G8" s="10">
-        <v>4860.32</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H8" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10">
         <v>5.0548260000000003</v>
-      </c>
-      <c r="I8" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="J8" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="L8" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="M8" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="N8" s="10" t="s">
+      <c r="M8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="10">
-        <v>81256680</v>
-      </c>
-      <c r="Q8" s="10">
+      <c r="N8" s="10">
         <v>2.7075819999999999</v>
       </c>
-      <c r="R8" s="10"/>
-      <c r="S8" s="6"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="6"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
     </row>
     <row r="9" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="10">
@@ -1118,39 +1116,32 @@
         <v>15360776</v>
       </c>
       <c r="G9" s="10">
-        <v>13622001</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H9" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I9" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J9" s="10">
-        <v>0.27730519999999997</v>
+        <v>4949128</v>
       </c>
       <c r="K9" s="10">
-        <v>4949128</v>
+        <v>3.1037340000000002</v>
       </c>
       <c r="L9" s="10">
         <v>3.1037340000000002</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10">
         <v>3.1037340000000002</v>
       </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>3.1037340000000002</v>
-      </c>
-      <c r="R9" s="10"/>
-      <c r="U9" s="4"/>
+      <c r="O9" s="10"/>
+      <c r="R9" s="4"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="10">
@@ -1166,39 +1157,35 @@
         <v>36277753.990000002</v>
       </c>
       <c r="G10" s="10">
-        <v>35186384</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H10" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I10" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J10" s="10">
-        <v>0.27730519999999997</v>
+        <v>22034940.920000002</v>
       </c>
       <c r="K10" s="10">
-        <v>22034940.920000002</v>
+        <v>1.646374</v>
       </c>
       <c r="L10" s="10">
         <v>1.646374</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="10"/>
+      <c r="N10" s="10">
         <v>1.646374</v>
       </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>1.646374</v>
-      </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="6"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="6"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="10">
@@ -1214,39 +1201,35 @@
         <v>658673</v>
       </c>
       <c r="G11" s="10">
-        <v>1040863</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H11" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I11" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J11" s="10">
-        <v>0.27730519999999997</v>
+        <v>255297.5</v>
       </c>
       <c r="K11" s="10">
-        <v>255297.5</v>
+        <v>2.5800209999999999</v>
       </c>
       <c r="L11" s="10">
         <v>2.5800209999999999</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="10"/>
+      <c r="N11" s="10">
         <v>2.5800209999999999</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="Q11" s="10">
-        <v>2.5800209999999999</v>
-      </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="6"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="6"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="10">
@@ -1262,39 +1245,35 @@
         <v>5140949</v>
       </c>
       <c r="G12" s="10">
-        <v>5214210</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H12" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I12" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J12" s="10">
-        <v>0.27730519999999997</v>
+        <v>2338974.5</v>
       </c>
       <c r="K12" s="10">
-        <v>2338974.5</v>
+        <v>2.1979500000000001</v>
       </c>
       <c r="L12" s="10">
         <v>2.1979500000000001</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="10"/>
+      <c r="N12" s="10">
         <v>2.1979500000000001</v>
       </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="Q12" s="10">
-        <v>2.1979500000000001</v>
-      </c>
-      <c r="R12" s="10"/>
-      <c r="S12" s="6"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="6"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="10">
@@ -1310,39 +1289,35 @@
         <v>5030867</v>
       </c>
       <c r="G13" s="10">
-        <v>6492255</v>
+        <v>5.0548260000000003</v>
       </c>
       <c r="H13" s="10">
-        <v>5.0548260000000003</v>
+        <v>54.853529999999999</v>
       </c>
       <c r="I13" s="10">
-        <v>54.853529999999999</v>
+        <v>0.27730519999999997</v>
       </c>
       <c r="J13" s="10">
-        <v>0.27730519999999997</v>
+        <v>669952</v>
       </c>
       <c r="K13" s="10">
-        <v>669952</v>
+        <v>7.5092949999999998</v>
       </c>
       <c r="L13" s="10">
         <v>7.5092949999999998</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="10"/>
+      <c r="N13" s="10">
         <v>7.5092949999999998</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>7.5092949999999998</v>
-      </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="6"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="6"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
     </row>
     <row r="14" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="10">
@@ -1357,44 +1332,37 @@
       <c r="F14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>1</v>
+      <c r="G14" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H14" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I14" s="10">
+      <c r="L14" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J14" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M14" s="10">
+      <c r="M14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="O14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="12"/>
-      <c r="P14" s="10">
-        <v>17962405</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="U14" s="4"/>
+      <c r="R14" s="4"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="10">
@@ -1409,44 +1377,40 @@
       <c r="F15" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>1</v>
+      <c r="G15" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H15" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I15" s="10">
+      <c r="L15" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J15" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M15" s="10">
+      <c r="M15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N15" s="10" t="s">
+      <c r="O15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="12"/>
-      <c r="P15" s="10">
-        <v>48157476</v>
-      </c>
-      <c r="Q15" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="10">
@@ -1461,44 +1425,40 @@
       <c r="F16" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>1</v>
+      <c r="G16" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H16" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I16" s="10">
+      <c r="L16" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J16" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M16" s="10">
+      <c r="M16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="O16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="12"/>
-      <c r="P16" s="10">
-        <v>59403681</v>
-      </c>
-      <c r="Q16" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+      <c r="P16" s="6"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="10">
@@ -1513,44 +1473,40 @@
       <c r="F17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>1</v>
+      <c r="G17" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H17" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I17" s="10">
+      <c r="L17" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J17" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M17" s="10">
+      <c r="M17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N17" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="O17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="12"/>
-      <c r="P17" s="10">
-        <v>70206081</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S17" s="6"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+      <c r="P17" s="6"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="10">
@@ -1565,55 +1521,51 @@
       <c r="F18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>1</v>
+      <c r="G18" s="10">
+        <v>5.0548260000000003</v>
       </c>
       <c r="H18" s="10">
+        <v>54.853529999999999</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.27730519999999997</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="10">
         <v>5.0548260000000003</v>
       </c>
-      <c r="I18" s="10">
+      <c r="L18" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="J18" s="10">
-        <v>0.27730519999999997</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="10">
-        <v>5.0548260000000003</v>
-      </c>
-      <c r="M18" s="10">
+      <c r="M18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="10">
         <v>54.853529999999999</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="O18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O18" s="12"/>
-      <c r="P18" s="10">
-        <v>70206307</v>
-      </c>
-      <c r="Q18" s="10">
-        <v>54.853529999999999</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S18" s="6"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="P18" s="6"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="21" t="s">
+      <c r="P21" s="13"/>
+      <c r="Q21" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="R21" s="26"/>
+      <c r="T21"/>
+      <c r="U21"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
@@ -1659,19 +1611,27 @@
       <c r="P22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" s="8" t="s">
+      <c r="Q22" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="T22" s="8" t="s">
+      <c r="R22" s="25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="S22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T22" t="s">
+        <v>80</v>
+      </c>
+      <c r="U22" t="s">
+        <v>77</v>
+      </c>
+      <c r="V22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="10">
@@ -1716,17 +1676,24 @@
       <c r="P23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="10">
-        <v>68047648</v>
-      </c>
-      <c r="S23" s="10">
+      <c r="Q23" s="10">
         <v>2.1466440000000002</v>
       </c>
-      <c r="T23" s="10"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="R23" s="10"/>
+      <c r="S23" s="2" t="e">
+        <f>G23/((D23+E23)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T23" s="2" t="e">
+        <f>H23/((E23+F23)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U23">
+        <v>0.96430340713054474</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="10">
@@ -1771,19 +1738,29 @@
       <c r="P24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="10">
-        <v>70206080</v>
-      </c>
-      <c r="S24" s="10">
+      <c r="Q24" s="10">
         <v>11.508599999999999</v>
       </c>
-      <c r="T24" s="10" t="s">
+      <c r="R24" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="S24" s="2" t="e">
+        <f t="shared" ref="S24:S27" si="0">G24/((D24+E24)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T24" s="2" t="e">
+        <f t="shared" ref="T24:T27" si="1">H24/((E24+F24)/1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U24">
+        <v>11.508599999999999</v>
+      </c>
+      <c r="V24" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="10">
@@ -1796,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="10">
-        <v>51000000</v>
+        <v>51</v>
       </c>
       <c r="G25" s="10">
         <v>95071</v>
@@ -1828,17 +1805,25 @@
       <c r="P25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="10">
-        <v>81256270</v>
-      </c>
-      <c r="S25" s="10">
+      <c r="Q25" s="10">
         <v>0.23152300000000001</v>
       </c>
-      <c r="T25" s="10"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="R25" s="10"/>
+      <c r="S25" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T25" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U25"/>
+      <c r="V25" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B26" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="10">
@@ -1883,17 +1868,24 @@
       <c r="P26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="10">
-        <v>81257338</v>
-      </c>
-      <c r="S26" s="10">
+      <c r="Q26" s="10">
         <v>2.8323559999999999</v>
       </c>
-      <c r="T26" s="10"/>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+      <c r="R26" s="10"/>
+      <c r="S26" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T26" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U26">
+        <v>0.28449832433210331</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B27" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="10">
@@ -1938,17 +1930,24 @@
       <c r="P27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="10">
-        <v>87962543</v>
-      </c>
-      <c r="S27" s="10">
+      <c r="Q27" s="10">
         <v>0.17911099999999999</v>
       </c>
-      <c r="T27" s="10"/>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="R27" s="10"/>
+      <c r="S27" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T27" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U27">
+        <v>-0.82824772620128728</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B28" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="10">
@@ -1991,17 +1990,28 @@
         <v>1.811755</v>
       </c>
       <c r="P28" s="10"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="S28" s="10">
-        <v>1.811755</v>
-      </c>
-      <c r="T28" s="10"/>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+      <c r="Q28" s="10">
+        <v>0.14397699999999999</v>
+      </c>
+      <c r="R28" s="10"/>
+      <c r="S28" s="2">
+        <f t="shared" ref="S28:S32" si="2">G28/((D28+E28)/2)</f>
+        <v>3.1037338294746064</v>
+      </c>
+      <c r="T28" s="2">
+        <f>H28/((E28+F28)/2)</f>
+        <v>2.7131086947018033</v>
+      </c>
+      <c r="U28">
+        <f t="shared" ref="U28:U32" si="3">S28/T28-1</f>
+        <v>0.14397695733149996</v>
+      </c>
+      <c r="W28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B29" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="10">
@@ -2044,17 +2054,28 @@
         <v>1.17293</v>
       </c>
       <c r="P29" s="10"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="S29" s="10">
-        <v>1.17293</v>
-      </c>
-      <c r="T29" s="10"/>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+      <c r="Q29" s="10">
+        <v>-0.31505</v>
+      </c>
+      <c r="R29" s="10"/>
+      <c r="S29" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6463740076140854</v>
+      </c>
+      <c r="T29" s="2">
+        <f t="shared" ref="T29:T32" si="4">H29/((E29+F29)/2)</f>
+        <v>2.4036424369644163</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="3"/>
+        <v>-0.31505036593824354</v>
+      </c>
+      <c r="W29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B30" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C30" s="10">
@@ -2097,17 +2118,28 @@
         <v>1.6497599999999999</v>
       </c>
       <c r="P30" s="10"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="S30" s="10">
-        <v>1.6497599999999999</v>
-      </c>
-      <c r="T30" s="10"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="Q30" s="10">
+        <v>6.2969999999999996E-3</v>
+      </c>
+      <c r="R30" s="10"/>
+      <c r="S30" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5800213476434357</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="4"/>
+        <v>2.5638771476652122</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="3"/>
+        <v>6.2967915576317424E-3</v>
+      </c>
+      <c r="W30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B31" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="10">
@@ -2150,17 +2182,28 @@
         <v>1.7427950000000001</v>
       </c>
       <c r="P31" s="10"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="S31" s="10">
-        <v>1.7427950000000001</v>
-      </c>
-      <c r="T31" s="10"/>
-    </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+      <c r="Q31" s="10">
+        <v>-2.7956000000000002E-2</v>
+      </c>
+      <c r="R31" s="10"/>
+      <c r="S31" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1979499990273514</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2611642864447763</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="3"/>
+        <v>-2.7956521247209598E-2</v>
+      </c>
+      <c r="W31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B32" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="10">
@@ -2203,17 +2246,28 @@
         <v>1.6762349999999999</v>
       </c>
       <c r="P32" s="10"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="S32" s="10">
-        <v>1.6762349999999999</v>
-      </c>
-      <c r="T32" s="10"/>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+      <c r="Q32" s="10">
+        <v>0.37034499999999998</v>
+      </c>
+      <c r="R32" s="10"/>
+      <c r="S32" s="2">
+        <f t="shared" si="2"/>
+        <v>7.5092946957393965</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="4"/>
+        <v>5.4798569148401901</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="3"/>
+        <v>0.37034503134620467</v>
+      </c>
+      <c r="W32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="10">
@@ -2258,19 +2312,16 @@
       <c r="P33" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="10">
-        <v>17962405</v>
-      </c>
-      <c r="S33" s="10">
-        <v>0</v>
-      </c>
-      <c r="T33" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="14" t="s">
+      <c r="Q33" s="10">
+        <v>0</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U33"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B34" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="10">
@@ -2315,19 +2366,16 @@
       <c r="P34" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="10">
-        <v>48157476</v>
-      </c>
-      <c r="S34" s="10">
-        <v>0</v>
-      </c>
-      <c r="T34" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+      <c r="Q34" s="10">
+        <v>0</v>
+      </c>
+      <c r="R34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U34"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B35" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C35" s="10">
@@ -2372,19 +2420,16 @@
       <c r="P35" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="10">
-        <v>59403681</v>
-      </c>
-      <c r="S35" s="10">
-        <v>0</v>
-      </c>
-      <c r="T35" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="Q35" s="10">
+        <v>0</v>
+      </c>
+      <c r="R35" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U35"/>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B36" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C36" s="10">
@@ -2429,19 +2474,16 @@
       <c r="P36" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="10">
-        <v>70206081</v>
-      </c>
-      <c r="S36" s="10">
-        <v>0</v>
-      </c>
-      <c r="T36" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+      <c r="Q36" s="10">
+        <v>0</v>
+      </c>
+      <c r="R36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U36"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B37" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C37" s="10">
@@ -2486,30 +2528,28 @@
       <c r="P37" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="10">
-        <v>70206307</v>
-      </c>
-      <c r="S37" s="10">
-        <v>0</v>
-      </c>
-      <c r="T37" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="Q37" s="10">
+        <v>0</v>
+      </c>
+      <c r="R37" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U37"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D40" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N40" s="21" t="s">
+      <c r="M40" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="16"/>
-      <c r="R40" s="16"/>
-    </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N40" s="26"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="T40"/>
+      <c r="U40"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>16</v>
       </c>
@@ -2543,21 +2583,19 @@
       <c r="L41" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M41" s="11"/>
-      <c r="N41" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O41" s="8" t="s">
+      <c r="M41" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="P41" s="8" t="s">
+      <c r="N41" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="T41"/>
+      <c r="U41"/>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C42" s="10">
@@ -2590,19 +2628,17 @@
       <c r="L42" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M42" s="11"/>
-      <c r="N42" s="10">
-        <v>27541053</v>
-      </c>
-      <c r="O42" s="10">
+      <c r="M42" s="10">
         <v>2.693085</v>
       </c>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="14" t="s">
+      <c r="N42" s="10"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="T42"/>
+      <c r="U42"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B43" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C43" s="10">
@@ -2635,19 +2671,17 @@
       <c r="L43" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="10">
-        <v>34457908</v>
-      </c>
-      <c r="O43" s="10">
+      <c r="M43" s="10">
         <v>105.300326</v>
       </c>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+      <c r="N43" s="10"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="T43"/>
+      <c r="U43"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B44" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="10">
@@ -2680,19 +2714,17 @@
       <c r="L44" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M44" s="11"/>
-      <c r="N44" s="10">
-        <v>52866669</v>
-      </c>
-      <c r="O44" s="10">
+      <c r="M44" s="10">
         <v>32.541947999999998</v>
       </c>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
+      <c r="N44" s="10"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="T44"/>
+      <c r="U44"/>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C45" s="10">
@@ -2725,19 +2757,17 @@
       <c r="L45" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M45" s="11"/>
-      <c r="N45" s="10">
-        <v>68047255</v>
-      </c>
-      <c r="O45" s="10">
+      <c r="M45" s="10">
         <v>3.2832210000000002</v>
       </c>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B46" s="14" t="s">
+      <c r="N45" s="10"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="T45"/>
+      <c r="U45"/>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B46" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="10">
@@ -2770,21 +2800,19 @@
       <c r="L46" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M46" s="11"/>
-      <c r="N46" s="10">
-        <v>68047613</v>
-      </c>
-      <c r="O46" s="10">
+      <c r="M46" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P46" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-    </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
+      <c r="N46" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="T46"/>
+      <c r="U46"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C47" s="10">
@@ -2815,19 +2843,17 @@
         <v>3.3743629999999998</v>
       </c>
       <c r="L47" s="10"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="O47" s="10">
+      <c r="M47" s="10">
         <v>3.3743629999999998</v>
       </c>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-    </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+      <c r="N47" s="10"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="T47"/>
+      <c r="U47"/>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B48" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C48" s="10">
@@ -2858,19 +2884,17 @@
         <v>6.3879580000000002</v>
       </c>
       <c r="L48" s="10"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="O48" s="10">
+      <c r="M48" s="10">
         <v>6.3879580000000002</v>
       </c>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
+      <c r="N48" s="10"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="T48"/>
+      <c r="U48"/>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B49" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C49" s="10">
@@ -2901,19 +2925,17 @@
         <v>2.5449679999999999</v>
       </c>
       <c r="L49" s="10"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="O49" s="10">
+      <c r="M49" s="10">
         <v>2.5449679999999999</v>
       </c>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-    </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
+      <c r="N49" s="10"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="T49"/>
+      <c r="U49"/>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B50" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="10">
@@ -2944,19 +2966,17 @@
         <v>14.894848</v>
       </c>
       <c r="L50" s="10"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="O50" s="10">
+      <c r="M50" s="10">
         <v>14.894848</v>
       </c>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-    </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
+      <c r="N50" s="10"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="T50"/>
+      <c r="U50"/>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B51" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C51" s="10">
@@ -2987,19 +3007,19 @@
         <v>3.6481370000000002</v>
       </c>
       <c r="L51" s="10"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="O51" s="10">
+      <c r="M51" s="10">
         <v>3.6481370000000002</v>
       </c>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-    </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="14"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="T51"/>
+      <c r="U51"/>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B52" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C52" s="10">
         <v>17962405</v>
       </c>
@@ -3030,21 +3050,21 @@
       <c r="L52" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M52" s="11"/>
-      <c r="N52" s="10">
-        <v>17962405</v>
-      </c>
-      <c r="O52" s="10">
+      <c r="M52" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P52" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-    </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B53" s="14"/>
+      <c r="N52" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="T52"/>
+      <c r="U52"/>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B53" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C53" s="10">
         <v>48157476</v>
       </c>
@@ -3075,21 +3095,21 @@
       <c r="L53" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M53" s="11"/>
-      <c r="N53" s="10">
-        <v>48157476</v>
-      </c>
-      <c r="O53" s="10">
+      <c r="M53" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P53" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-    </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="14"/>
+      <c r="N53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="T53"/>
+      <c r="U53"/>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B54" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C54" s="10">
         <v>59403681</v>
       </c>
@@ -3120,21 +3140,21 @@
       <c r="L54" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M54" s="11"/>
-      <c r="N54" s="10">
-        <v>59403681</v>
-      </c>
-      <c r="O54" s="10">
+      <c r="M54" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P54" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="11"/>
-    </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B55" s="14"/>
+      <c r="N54" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="T54"/>
+      <c r="U54"/>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B55" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C55" s="10">
         <v>68047257</v>
       </c>
@@ -3165,21 +3185,21 @@
       <c r="L55" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M55" s="11"/>
-      <c r="N55" s="10">
-        <v>68047257</v>
-      </c>
-      <c r="O55" s="10">
+      <c r="M55" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P55" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-    </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="14"/>
+      <c r="N55" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="T55"/>
+      <c r="U55"/>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B56" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="C56" s="10">
         <v>70206081</v>
       </c>
@@ -3210,40 +3230,37 @@
       <c r="L56" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M56" s="11"/>
-      <c r="N56" s="10">
-        <v>70206081</v>
-      </c>
-      <c r="O56" s="10">
+      <c r="M56" s="10">
         <v>7.1190810000000004</v>
       </c>
-      <c r="P56" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-    </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="T56"/>
+      <c r="U56"/>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="P57" s="5"/>
       <c r="Q57" s="5"/>
       <c r="R57" s="5"/>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
       <c r="R58" s="5"/>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D59" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U59" s="21" t="s">
+      <c r="T59" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="V59" s="21"/>
-      <c r="W59" s="21"/>
-    </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U59" s="26"/>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B60" s="9" t="s">
         <v>16</v>
       </c>
@@ -3298,18 +3315,15 @@
       <c r="S60" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="U60" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V60" s="8" t="s">
+      <c r="T60" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="W60" s="8" t="s">
+      <c r="U60" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B61" s="14" t="s">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B61" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C61" s="10">
@@ -3363,16 +3377,13 @@
       <c r="S61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U61" s="10">
-        <v>27541053</v>
-      </c>
-      <c r="V61" s="10">
+      <c r="T61" s="10">
         <v>-0.86645000000000005</v>
       </c>
-      <c r="W61" s="10"/>
-    </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B62" s="14" t="s">
+      <c r="U61" s="10"/>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B62" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C62" s="10">
@@ -3426,16 +3437,13 @@
       <c r="S62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U62" s="10">
-        <v>70206124</v>
-      </c>
-      <c r="V62" s="10">
+      <c r="T62" s="10">
         <v>-0.88441499999999995</v>
       </c>
-      <c r="W62" s="10"/>
-    </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B63" s="14" t="s">
+      <c r="U62" s="10"/>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B63" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C63" s="10">
@@ -3489,16 +3497,13 @@
       <c r="S63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U63" s="10">
-        <v>81256268</v>
-      </c>
-      <c r="V63" s="10">
+      <c r="T63" s="10">
         <v>1.743474</v>
       </c>
-      <c r="W63" s="10"/>
-    </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B64" s="14" t="s">
+      <c r="U63" s="10"/>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B64" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C64" s="10">
@@ -3552,16 +3557,13 @@
       <c r="S64" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U64" s="10">
-        <v>81256616</v>
-      </c>
-      <c r="V64" s="10">
+      <c r="T64" s="10">
         <v>12.61281</v>
       </c>
-      <c r="W64" s="10"/>
-    </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B65" s="14" t="s">
+      <c r="U64" s="10"/>
+    </row>
+    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B65" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C65" s="10">
@@ -3615,16 +3617,13 @@
       <c r="S65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U65" s="10">
-        <v>81256724</v>
-      </c>
-      <c r="V65" s="10">
+      <c r="T65" s="10">
         <v>1.225859</v>
       </c>
-      <c r="W65" s="10"/>
-    </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B66" s="14" t="s">
+      <c r="U65" s="10"/>
+    </row>
+    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B66" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C66" s="10">
@@ -3676,16 +3675,13 @@
         <v>0.81800799999999996</v>
       </c>
       <c r="S66" s="1"/>
-      <c r="U66" s="10">
-        <v>17959726</v>
-      </c>
-      <c r="V66" s="1">
+      <c r="T66" s="1">
         <v>0.81800799999999996</v>
       </c>
-      <c r="W66" s="1"/>
-    </row>
-    <row r="67" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B67" s="14" t="s">
+      <c r="U66" s="1"/>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B67" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C67" s="10">
@@ -3737,16 +3733,13 @@
         <v>0.12714</v>
       </c>
       <c r="S67" s="1"/>
-      <c r="U67" s="10">
-        <v>17993020</v>
-      </c>
-      <c r="V67" s="1">
+      <c r="T67" s="1">
         <v>0.12714</v>
       </c>
-      <c r="W67" s="1"/>
-    </row>
-    <row r="68" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B68" s="14" t="s">
+      <c r="U67" s="1"/>
+    </row>
+    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B68" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C68" s="10">
@@ -3798,16 +3791,13 @@
         <v>-0.396013</v>
       </c>
       <c r="S68" s="1"/>
-      <c r="U68" s="10">
-        <v>26852786</v>
-      </c>
-      <c r="V68" s="1">
+      <c r="T68" s="1">
         <v>-0.396013</v>
       </c>
-      <c r="W68" s="1"/>
-    </row>
-    <row r="69" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B69" s="14" t="s">
+      <c r="U68" s="1"/>
+    </row>
+    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B69" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C69" s="10">
@@ -3859,16 +3849,13 @@
         <v>0.27766600000000002</v>
       </c>
       <c r="S69" s="1"/>
-      <c r="U69" s="10">
-        <v>26852818</v>
-      </c>
-      <c r="V69" s="1">
+      <c r="T69" s="1">
         <v>0.27766600000000002</v>
       </c>
-      <c r="W69" s="1"/>
-    </row>
-    <row r="70" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B70" s="14" t="s">
+      <c r="U69" s="1"/>
+    </row>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B70" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C70" s="10">
@@ -3920,25 +3907,22 @@
         <v>0.262847</v>
       </c>
       <c r="S70" s="1"/>
-      <c r="U70" s="10">
-        <v>26852821</v>
-      </c>
-      <c r="V70" s="1">
+      <c r="T70" s="1">
         <v>0.262847</v>
       </c>
-      <c r="W70" s="1"/>
-    </row>
-    <row r="71" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B71" s="14" t="s">
+      <c r="U70" s="1"/>
+    </row>
+    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B71" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C71" s="10">
         <v>27853141</v>
       </c>
-      <c r="D71" s="25">
+      <c r="D71" s="22">
         <v>92858</v>
       </c>
-      <c r="E71" s="25">
+      <c r="E71" s="22">
         <v>96325</v>
       </c>
       <c r="F71" s="10" t="s">
@@ -3956,22 +3940,22 @@
       <c r="J71" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K71" s="26">
+      <c r="K71" s="23">
         <v>92858</v>
       </c>
-      <c r="L71" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M71" s="26">
+      <c r="L71" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M71" s="23">
         <v>96325</v>
       </c>
-      <c r="N71" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O71" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P71" s="27" t="s">
+      <c r="N71" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O71" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P71" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q71" s="1">
@@ -3980,30 +3964,27 @@
       <c r="R71" s="1">
         <v>0</v>
       </c>
-      <c r="S71" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U71" s="10">
-        <v>27853141</v>
-      </c>
-      <c r="V71" s="1">
-        <v>0</v>
-      </c>
-      <c r="W71" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B72" s="14" t="s">
+      <c r="S71" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T71" s="1">
+        <v>0</v>
+      </c>
+      <c r="U71" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B72" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C72" s="10">
         <v>27853308</v>
       </c>
-      <c r="D72" s="25">
+      <c r="D72" s="22">
         <v>224506</v>
       </c>
-      <c r="E72" s="25">
+      <c r="E72" s="22">
         <v>146182</v>
       </c>
       <c r="F72" s="10" t="s">
@@ -4021,22 +4002,22 @@
       <c r="J72" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K72" s="26">
+      <c r="K72" s="23">
         <v>224506</v>
       </c>
-      <c r="L72" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M72" s="26">
+      <c r="L72" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M72" s="23">
         <v>146182</v>
       </c>
-      <c r="N72" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O72" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P72" s="27" t="s">
+      <c r="N72" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O72" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P72" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q72" s="1">
@@ -4045,30 +4026,27 @@
       <c r="R72" s="1">
         <v>0</v>
       </c>
-      <c r="S72" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U72" s="10">
-        <v>27853308</v>
-      </c>
-      <c r="V72" s="1">
-        <v>0</v>
-      </c>
-      <c r="W72" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B73" s="14" t="s">
+      <c r="S72" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T72" s="1">
+        <v>0</v>
+      </c>
+      <c r="U72" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B73" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C73" s="10">
         <v>68047770</v>
       </c>
-      <c r="D73" s="25">
+      <c r="D73" s="22">
         <v>1678951</v>
       </c>
-      <c r="E73" s="25">
+      <c r="E73" s="22">
         <v>1408373</v>
       </c>
       <c r="F73" s="10" t="s">
@@ -4086,22 +4064,22 @@
       <c r="J73" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K73" s="26">
+      <c r="K73" s="23">
         <v>1678951</v>
       </c>
-      <c r="L73" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M73" s="26">
+      <c r="L73" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M73" s="23">
         <v>1408373</v>
       </c>
-      <c r="N73" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O73" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P73" s="27" t="s">
+      <c r="N73" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O73" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P73" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q73" s="1">
@@ -4110,30 +4088,27 @@
       <c r="R73" s="1">
         <v>0</v>
       </c>
-      <c r="S73" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U73" s="10">
-        <v>68047770</v>
-      </c>
-      <c r="V73" s="1">
-        <v>0</v>
-      </c>
-      <c r="W73" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B74" s="14" t="s">
+      <c r="S73" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T73" s="1">
+        <v>0</v>
+      </c>
+      <c r="U73" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B74" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C74" s="10">
         <v>68048348</v>
       </c>
-      <c r="D74" s="25">
+      <c r="D74" s="22">
         <v>32873</v>
       </c>
-      <c r="E74" s="25">
+      <c r="E74" s="22">
         <v>45195.5</v>
       </c>
       <c r="F74" s="10" t="s">
@@ -4151,22 +4126,22 @@
       <c r="J74" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K74" s="26">
+      <c r="K74" s="23">
         <v>32873</v>
       </c>
-      <c r="L74" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M74" s="26">
+      <c r="L74" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M74" s="23">
         <v>45195.5</v>
       </c>
-      <c r="N74" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O74" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P74" s="27" t="s">
+      <c r="N74" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O74" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P74" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q74" s="1">
@@ -4175,30 +4150,27 @@
       <c r="R74" s="1">
         <v>0</v>
       </c>
-      <c r="S74" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U74" s="10">
-        <v>68048348</v>
-      </c>
-      <c r="V74" s="1">
-        <v>0</v>
-      </c>
-      <c r="W74" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B75" s="14" t="s">
+      <c r="S74" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T74" s="1">
+        <v>0</v>
+      </c>
+      <c r="U74" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B75" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C75" s="10">
         <v>81256246</v>
       </c>
-      <c r="D75" s="25">
+      <c r="D75" s="22">
         <v>364466</v>
       </c>
-      <c r="E75" s="25">
+      <c r="E75" s="22">
         <v>269600</v>
       </c>
       <c r="F75" s="10" t="s">
@@ -4216,22 +4188,22 @@
       <c r="J75" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K75" s="26">
+      <c r="K75" s="23">
         <v>364466</v>
       </c>
-      <c r="L75" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M75" s="26">
+      <c r="L75" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M75" s="23">
         <v>269600</v>
       </c>
-      <c r="N75" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O75" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="P75" s="27" t="s">
+      <c r="N75" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O75" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P75" s="24" t="s">
         <v>1</v>
       </c>
       <c r="Q75" s="1">
@@ -4240,30 +4212,28 @@
       <c r="R75" s="1">
         <v>0</v>
       </c>
-      <c r="S75" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="U75" s="10">
-        <v>81256246</v>
-      </c>
-      <c r="V75" s="1">
-        <v>0</v>
-      </c>
-      <c r="W75" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="S75" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="T75" s="1">
+        <v>0</v>
+      </c>
+      <c r="U75" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N78" s="21" t="s">
+      <c r="M78" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="O78" s="21"/>
-      <c r="P78" s="21"/>
-    </row>
-    <row r="79" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N78" s="26"/>
+      <c r="T78"/>
+      <c r="U78"/>
+    </row>
+    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B79" s="9" t="s">
         <v>16</v>
       </c>
@@ -4297,31 +4267,33 @@
       <c r="L79" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="M79" s="11"/>
-      <c r="N79" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O79" s="8" t="s">
+      <c r="M79" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="P79" s="8" t="s">
+      <c r="N79" s="25" t="s">
         <v>62</v>
       </c>
+      <c r="O79" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P79" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="Q79" s="11"/>
-      <c r="R79" s="11"/>
-      <c r="S79" s="11"/>
-    </row>
-    <row r="80" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B80" s="14" t="s">
+      <c r="T79"/>
+      <c r="U79"/>
+    </row>
+    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B80" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D80" s="17">
+      <c r="D80" s="15">
         <v>10</v>
       </c>
-      <c r="E80" s="17">
+      <c r="E80" s="15">
         <v>500</v>
       </c>
       <c r="F80" s="10" t="s">
@@ -4336,36 +4308,41 @@
       <c r="I80" s="10">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J80" s="17">
+      <c r="J80" s="15">
         <v>50</v>
       </c>
-      <c r="K80" s="17">
+      <c r="K80" s="15">
         <v>50</v>
       </c>
       <c r="L80" s="10"/>
-      <c r="M80" s="11"/>
+      <c r="M80" s="10">
+        <v>50</v>
+      </c>
       <c r="N80" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="O80" s="10">
-        <v>50</v>
-      </c>
-      <c r="P80" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="O80" s="5" t="e">
+        <f>(E80+F80)/D80</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P80" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-      <c r="S80" s="5"/>
-    </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B81" s="14" t="s">
+      <c r="T80"/>
+      <c r="U80"/>
+    </row>
+    <row r="81" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B81" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D81" s="17">
+      <c r="D81" s="15">
         <v>10</v>
       </c>
-      <c r="E81" s="17">
+      <c r="E81" s="15">
         <v>500</v>
       </c>
       <c r="F81" s="10" t="s">
@@ -4374,49 +4351,51 @@
       <c r="G81" s="10">
         <v>0.74209000000000003</v>
       </c>
-      <c r="H81" s="19">
+      <c r="H81" s="17">
         <v>1.7168680000000001</v>
       </c>
       <c r="I81" s="10">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J81" s="17">
+      <c r="J81" s="15">
         <v>50</v>
       </c>
-      <c r="K81" s="19">
+      <c r="K81" s="17">
         <v>1.7168680000000001</v>
       </c>
       <c r="L81" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="M81" s="11"/>
+      <c r="M81" s="10">
+        <v>1.7168680000000001</v>
+      </c>
       <c r="N81" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="O81" s="10">
+        <v>68</v>
+      </c>
+      <c r="O81" s="5">
         <v>1.7168680000000001</v>
       </c>
       <c r="P81" s="10" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
-      <c r="S81" s="5"/>
-    </row>
-    <row r="82" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B82" s="10" t="s">
+      <c r="T81"/>
+      <c r="U81"/>
+    </row>
+    <row r="82" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B82" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D82" s="17">
+      <c r="D82" s="15">
         <v>10</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F82" s="18">
+      <c r="F82" s="16">
         <v>800</v>
       </c>
       <c r="G82" s="1">
@@ -4428,69 +4407,74 @@
       <c r="I82" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J82" s="18">
+      <c r="J82" s="16">
         <v>80</v>
       </c>
-      <c r="K82" s="18">
+      <c r="K82" s="16">
         <v>80</v>
       </c>
       <c r="L82" s="1"/>
-      <c r="N82" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="O82" s="1">
+      <c r="M82" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="P82" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B83" s="10" t="s">
+      <c r="N82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O82" s="5"/>
+      <c r="T82"/>
+      <c r="U82"/>
+    </row>
+    <row r="83" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B83" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D83" s="17">
+      <c r="D83" s="15">
         <v>10</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F83" s="18">
+      <c r="F83" s="16">
         <v>800</v>
       </c>
       <c r="G83" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="H83" s="20">
+      <c r="H83" s="18">
         <v>1.7168680000000001</v>
       </c>
       <c r="I83" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J83" s="18">
+      <c r="J83" s="16">
         <v>80</v>
       </c>
-      <c r="K83" s="20">
+      <c r="K83" s="18">
         <v>1.7168680000000001</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N83" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="O83" s="1">
+      <c r="M83" s="1">
         <v>0.74209000000000003</v>
       </c>
+      <c r="N83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O83" s="5">
+        <v>0.74209000000000003</v>
+      </c>
       <c r="P83" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B84" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="T83"/>
+      <c r="U83"/>
+    </row>
+    <row r="84" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B84" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -4523,18 +4507,16 @@
       <c r="L84" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N84" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="O84" s="1">
-        <v>1.7168680000000001</v>
-      </c>
-      <c r="P84" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B85" s="10" t="s">
+      <c r="M84" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="N84" s="1"/>
+      <c r="O84" s="5"/>
+      <c r="T84"/>
+      <c r="U84"/>
+    </row>
+    <row r="85" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B85" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -4567,18 +4549,16 @@
       <c r="L85" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N85" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="O85" s="1">
-        <v>1.7168680000000001</v>
-      </c>
-      <c r="P85" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B86" s="10" t="s">
+      <c r="M85" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="N85" s="1"/>
+      <c r="O85" s="5"/>
+      <c r="T85"/>
+      <c r="U85"/>
+    </row>
+    <row r="86" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B86" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -4611,18 +4591,18 @@
       <c r="L86" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N86" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O86" s="1">
+      <c r="M86" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="P86" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B87" s="10" t="s">
+      <c r="N86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O86" s="5"/>
+      <c r="T86"/>
+      <c r="U86"/>
+    </row>
+    <row r="87" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B87" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -4655,27 +4635,27 @@
       <c r="L87" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N87" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O87" s="1">
+      <c r="M87" s="1">
         <v>0.74209000000000003</v>
       </c>
-      <c r="P87" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B88" s="10" t="s">
+      <c r="N87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O87" s="5"/>
+      <c r="T87"/>
+      <c r="U87"/>
+    </row>
+    <row r="88" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B88" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D88" s="18">
+      <c r="D88" s="16">
         <v>500</v>
       </c>
-      <c r="E88" s="18">
+      <c r="E88" s="16">
         <v>10</v>
       </c>
       <c r="F88" s="1" t="s">
@@ -4690,7 +4670,7 @@
       <c r="I88" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J88" s="18">
+      <c r="J88" s="16">
         <v>50</v>
       </c>
       <c r="K88" s="1">
@@ -4699,27 +4679,32 @@
       <c r="L88" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N88" s="10" t="s">
-        <v>73</v>
+      <c r="M88" s="1">
+        <v>6.9793999999999995E-2</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="O88" s="1">
-        <v>1.7168680000000001</v>
-      </c>
-      <c r="P88" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B89" s="10" t="s">
+        <v>6.9793999999999995E-2</v>
+      </c>
+      <c r="P88" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="T88"/>
+      <c r="U88"/>
+    </row>
+    <row r="89" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B89" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D89" s="18">
+      <c r="D89" s="16">
         <v>500</v>
       </c>
-      <c r="E89" s="18">
+      <c r="E89" s="16">
         <v>10</v>
       </c>
       <c r="F89" s="1" t="s">
@@ -4734,7 +4719,7 @@
       <c r="I89" s="1">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="J89" s="18">
+      <c r="J89" s="16">
         <v>50</v>
       </c>
       <c r="K89" s="1">
@@ -4743,23 +4728,28 @@
       <c r="L89" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N89" s="10" t="s">
-        <v>74</v>
+      <c r="M89" s="1">
+        <v>6.9793999999999995E-2</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="O89" s="1">
-        <v>1.7168680000000001</v>
-      </c>
-      <c r="P89" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>6.9793999999999995E-2</v>
+      </c>
+      <c r="P89" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="T89"/>
+      <c r="U89"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="U59:W59"/>
-    <mergeCell ref="N78:P78"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="T59:U59"/>
+    <mergeCell ref="M78:N78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4800,200 +4790,200 @@
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="19">
         <v>500</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="19">
         <v>10</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="19">
         <v>800</v>
       </c>
       <c r="F3">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H3">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="19">
         <v>130</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="K3" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="19">
         <v>500</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="19">
         <v>10</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="19">
         <v>800</v>
       </c>
       <c r="F4">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H4">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="19">
         <v>130</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="19">
         <v>500</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="19">
         <v>10</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="19">
         <v>800</v>
       </c>
       <c r="F5">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H5">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="19">
         <v>130</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="19">
         <v>500</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="19">
         <v>10</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="19">
         <v>800</v>
       </c>
       <c r="F6">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H6">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="19">
         <v>130</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="K6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="19">
         <v>500</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="19">
         <v>10</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="19">
         <v>800</v>
       </c>
       <c r="F7">
         <v>0.74209000000000003</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>1.7168680000000001</v>
       </c>
       <c r="H7">
         <v>6.9793999999999995E-2</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="19">
         <v>130</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="20">
         <v>1.7168680000000001</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aggiunto separatore ; per gli errori sull'indicatore 56
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_syt.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="84">
   <si>
     <t>SNDG</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>err_atteso</t>
+  </si>
+  <si>
+    <t>E0003;E0002;</t>
   </si>
 </sst>
 </file>
@@ -778,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="L58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N82" sqref="N82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4370,7 +4373,7 @@
         <v>1.7168680000000001</v>
       </c>
       <c r="N81" s="10" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="O81" s="5">
         <v>1.7168680000000001</v>

</xml_diff>